<commit_message>
Se cambio a los correos que venian predenterminados.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\Asiganción NS\FreFramework-Excel\FreFramework-Excel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936B8519-419D-49AE-BF08-3B7789C0C3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60B0E17-9D3E-456A-91BB-A5714C72CDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -271,10 +271,10 @@
     <t>Solicitud de vale</t>
   </si>
   <si>
-    <t>carlos.bautista@ipiam.edu.mx</t>
-  </si>
-  <si>
     <t>https://cloud.uipath.com/vwkynps/DefaultTenant/orchestrator_/?tid=1121059&amp;fid=3426244</t>
+  </si>
+  <si>
+    <t>luis.ramos@beeckerco.com</t>
   </si>
 </sst>
 </file>
@@ -1838,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1988,7 +1988,7 @@
         <v>52</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>53</v>
@@ -2021,7 +2021,7 @@
         <v>59</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>60</v>
@@ -3138,7 +3138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>